<commit_message>
Se agrega rutinas para reclasificacion de Flores, Beechie, Qmax, Lang
</commit_message>
<xml_diff>
--- a/Check_For_Cluster.xlsx
+++ b/Check_For_Cluster.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria.vieira\Box Sync\MIV\Dulceacuícola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\MCAD\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B031865D-B806-4DEC-860C-2752D7E03195}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84C0CA8-874C-464A-9114-53E75CECFF44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{B166D140-3300-45F9-827E-0E6C55D0D5B0}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{B166D140-3300-45F9-827E-0E6C55D0D5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="oct 9" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="135">
   <si>
     <t>Marino Costeros</t>
   </si>
@@ -323,6 +330,114 @@
   </si>
   <si>
     <t>Categoría final</t>
+  </si>
+  <si>
+    <t>BAJO</t>
+  </si>
+  <si>
+    <t>ALTO</t>
+  </si>
+  <si>
+    <t>Formas de lecho - FLORES</t>
+  </si>
+  <si>
+    <t>MEDIO BAJO</t>
+  </si>
+  <si>
+    <t>MEDIO ALTO</t>
+  </si>
+  <si>
+    <t>&gt; 75</t>
+  </si>
+  <si>
+    <t>Calido Humedo</t>
+  </si>
+  <si>
+    <t>Calido Semihumedo</t>
+  </si>
+  <si>
+    <t>Calido Arido</t>
+  </si>
+  <si>
+    <t>Frio Humedo</t>
+  </si>
+  <si>
+    <t>Calido Superhumedo</t>
+  </si>
+  <si>
+    <t>Muy frio Semihumedo</t>
+  </si>
+  <si>
+    <t>Templado Semiarido</t>
+  </si>
+  <si>
+    <t>Frio Semihumedo</t>
+  </si>
+  <si>
+    <t>Frio Semiarido</t>
+  </si>
+  <si>
+    <t>Frio Superhumedo</t>
+  </si>
+  <si>
+    <t>Calido Semiarido</t>
+  </si>
+  <si>
+    <t>Muy frio Humedo</t>
+  </si>
+  <si>
+    <t>Muy frio Superhumedo</t>
+  </si>
+  <si>
+    <t>Calido Desertico</t>
+  </si>
+  <si>
+    <t>Templado Semihumedo</t>
+  </si>
+  <si>
+    <t>Templado Humedo</t>
+  </si>
+  <si>
+    <t>Templado Superhumedo</t>
+  </si>
+  <si>
+    <t>Extremadamente frio Superhumedo</t>
+  </si>
+  <si>
+    <t>Extremadamente frio Humedo</t>
+  </si>
+  <si>
+    <t>Frio Arido</t>
+  </si>
+  <si>
+    <t>Nival Superhumedo</t>
+  </si>
+  <si>
+    <t>Muy frio Semiarido</t>
+  </si>
+  <si>
+    <t>Templado Arido</t>
+  </si>
+  <si>
+    <t>Calido seco</t>
+  </si>
+  <si>
+    <t>Calido humedo</t>
+  </si>
+  <si>
+    <t>Templado humedo</t>
+  </si>
+  <si>
+    <t>Muy Frio humedo</t>
+  </si>
+  <si>
+    <t>Frio humedo</t>
+  </si>
+  <si>
+    <t>Frio Seco</t>
+  </si>
+  <si>
+    <t>Frio arido</t>
   </si>
 </sst>
 </file>
@@ -354,12 +469,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -524,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,74 +669,128 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,7 +810,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -932,7 +1113,7 @@
       <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -941,11 +1122,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,622 +1139,617 @@
       <c r="C3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="24"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="24"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="25"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="18"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="12"/>
+      <c r="D22" s="14"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="13"/>
+      <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="12"/>
+      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="12"/>
+      <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="13"/>
+      <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="2"/>
       <c r="C30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="12"/>
+      <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="2"/>
       <c r="C31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="2"/>
       <c r="C32" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="2"/>
       <c r="C33" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="2"/>
       <c r="C34" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="13"/>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="2"/>
       <c r="C35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="12"/>
+      <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="2"/>
       <c r="C36" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="2"/>
       <c r="C37" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="2"/>
       <c r="C38" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="13" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="2"/>
       <c r="C39" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="12"/>
+      <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="2"/>
       <c r="C40" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="2"/>
       <c r="C41" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="12"/>
+      <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="2"/>
       <c r="C42" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="2"/>
       <c r="C43" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="12"/>
+      <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="2"/>
       <c r="C44" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="9" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="2"/>
       <c r="C45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="2"/>
       <c r="C46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="13"/>
+      <c r="D46" s="18"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="2"/>
       <c r="C47" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="12"/>
+      <c r="D47" s="14"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="19" t="s">
+      <c r="A48" s="26"/>
+      <c r="B48" s="27" t="s">
         <v>55</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D48" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="19"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="27"/>
       <c r="C49" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="13"/>
+      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="19"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="12"/>
+      <c r="D50" s="14"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
       <c r="C52" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="8"/>
+      <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="8"/>
+      <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D54" s="8"/>
+      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="20"/>
       <c r="C55" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D55" s="8"/>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
       <c r="C56" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D56" s="8"/>
+      <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="8"/>
+      <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="21"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="23"/>
       <c r="C58" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="8"/>
+      <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="22"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D59" s="8"/>
+      <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="B60" s="16" t="s">
+      <c r="A60" s="20"/>
+      <c r="B60" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="8"/>
+      <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
+      <c r="A61" s="20"/>
+      <c r="B61" s="20"/>
       <c r="C61" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="8"/>
+      <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="20"/>
       <c r="C62" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D62" s="8"/>
+      <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
       <c r="C63" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D63" s="8"/>
+      <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="19" t="s">
         <v>60</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="8"/>
+      <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
       <c r="C65" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D65" s="8"/>
+      <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
       <c r="C66" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D66" s="8"/>
+      <c r="D66" s="7"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
       <c r="C67" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="8"/>
+      <c r="D67" s="7"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="17"/>
-      <c r="B68" s="18"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="21"/>
       <c r="C68" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D68" s="8"/>
+      <c r="D68" s="7"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="16" t="s">
+      <c r="A69" s="20"/>
+      <c r="B69" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D69" s="8"/>
+      <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
       <c r="C70" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D70" s="9"/>
+      <c r="D70" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D3:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A64:A70"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B9:B16"/>
@@ -1586,13 +1762,18 @@
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A64:A70"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D3:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1601,27 +1782,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8817F625-8B1F-4646-88EB-C81E20F52766}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="B18:D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1633,145 +1814,145 @@
       <c r="C3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="30" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1785,397 +1966,421 @@
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="38" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="31"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="38"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="31"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="19"/>
+      <c r="D20" s="38"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="31"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="38" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="31"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="19"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="31"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="38"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="4" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="38" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="19"/>
+      <c r="D25" s="38"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="4" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="38" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="5" t="s">
+      <c r="A27" s="31"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="38"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="5" t="s">
+      <c r="A28" s="31"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="19"/>
+      <c r="D28" s="38"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="5" t="s">
+      <c r="A29" s="31"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="38" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="5" t="s">
+      <c r="A30" s="31"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="38"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="5" t="s">
+      <c r="A31" s="31"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="38" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="5" t="s">
+      <c r="A32" s="31"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="5" t="s">
+      <c r="A33" s="31"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="5" t="s">
+      <c r="A34" s="31"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="38" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="5" t="s">
+      <c r="A35" s="31"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="5" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="38" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="5" t="s">
+      <c r="A37" s="31"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="19"/>
+      <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="5" t="s">
+      <c r="A38" s="31"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="38" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="5" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="19"/>
+      <c r="D39" s="38"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="5" t="s">
+      <c r="A40" s="31"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="38" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="5" t="s">
+      <c r="A41" s="31"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="19"/>
+      <c r="D41" s="38"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="5" t="s">
+      <c r="A42" s="31"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="36" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="5" t="s">
+      <c r="A43" s="31"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="38" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="5" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="19"/>
+      <c r="D44" s="38"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="5" t="s">
+      <c r="A45" s="31"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="19"/>
+      <c r="D45" s="38"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="38" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="4" t="s">
+      <c r="A47" s="20"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="19"/>
+      <c r="D47" s="38"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="4" t="s">
+      <c r="A48" s="20"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="19"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="16" t="s">
+      <c r="D48" s="38"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="29" t="s">
+      <c r="C49" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="39" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="29"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="29"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="29"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="E49">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D50" s="39"/>
+      <c r="E50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="39"/>
+      <c r="E51">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="39"/>
+      <c r="E52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="4" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="38" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="4" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="20"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="19"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="4" t="s">
+      <c r="D55" s="38"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="19"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="4" t="s">
+      <c r="D56" s="38"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="20"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D57" s="19"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C58" s="4" t="s">
+      <c r="D57" s="38"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="20"/>
+      <c r="B58" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D58" s="28" t="s">
+      <c r="D58" s="30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="4" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D59" s="28" t="s">
+      <c r="D59" s="30" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B59"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D43:D45"/>
@@ -2189,17 +2394,396 @@
     <mergeCell ref="D31:D33"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="B9:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F028EF4D-E687-468B-B356-5AD629E8C333}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ajustes funcion beechie y add_attibute exportacion de tablas en formato csv
</commit_message>
<xml_diff>
--- a/Check_For_Cluster.xlsx
+++ b/Check_For_Cluster.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\MCAD\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84C0CA8-874C-464A-9114-53E75CECFF44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26535896-1670-4693-AC99-74458AB6DB11}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{B166D140-3300-45F9-827E-0E6C55D0D5B0}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{B166D140-3300-45F9-827E-0E6C55D0D5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="oct 9" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="135">
   <si>
     <t>Marino Costeros</t>
   </si>
@@ -687,82 +688,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -777,6 +712,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -786,8 +778,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1109,7 +1110,7 @@
   <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -1122,11 +1123,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,368 +1140,368 @@
       <c r="C3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="37" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="38"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="38"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="38"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="38"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="16"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="38"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="38"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="38"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="38"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="38"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="38"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="17"/>
+      <c r="D19" s="39"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="29" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="25" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="18"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="25" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="18"/>
+      <c r="D24" s="27"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="14"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="25" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="18"/>
+      <c r="D29" s="27"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="2"/>
       <c r="C30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="14"/>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="2"/>
       <c r="C31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="25" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="2"/>
       <c r="C32" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="14"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="2"/>
       <c r="C33" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="25" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="2"/>
       <c r="C34" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="27"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="2"/>
       <c r="C35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="14"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="2"/>
       <c r="C36" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="25" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="2"/>
       <c r="C37" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="14"/>
+      <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="2"/>
       <c r="C38" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="25" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="2"/>
       <c r="C39" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="26"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="2"/>
       <c r="C40" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="25" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="2"/>
       <c r="C41" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="14"/>
+      <c r="D41" s="26"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="2"/>
       <c r="C42" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="25" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="2"/>
       <c r="C43" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="14"/>
+      <c r="D43" s="26"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="2"/>
       <c r="C44" s="5" t="s">
         <v>79</v>
@@ -1510,64 +1511,64 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="2"/>
       <c r="C45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="25" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="2"/>
       <c r="C46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="18"/>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="2"/>
       <c r="C47" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="14"/>
+      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
-      <c r="B48" s="27" t="s">
+      <c r="A48" s="29"/>
+      <c r="B48" s="33" t="s">
         <v>55</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="33"/>
       <c r="C49" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="18"/>
+      <c r="D49" s="27"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="14"/>
+      <c r="D50" s="26"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="30" t="s">
         <v>44</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -1578,50 +1579,50 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
-      <c r="B56" s="21"/>
+      <c r="A56" s="32"/>
+      <c r="B56" s="32"/>
       <c r="C56" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="34" t="s">
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -1630,24 +1631,24 @@
       <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
-      <c r="B58" s="23"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="35"/>
       <c r="C58" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
-      <c r="B59" s="24"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="36"/>
       <c r="C59" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
-      <c r="B60" s="19" t="s">
+      <c r="A60" s="31"/>
+      <c r="B60" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -1656,34 +1657,34 @@
       <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
-      <c r="B62" s="20"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="31"/>
       <c r="C62" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="21"/>
-      <c r="B63" s="21"/>
+      <c r="A63" s="32"/>
+      <c r="B63" s="32"/>
       <c r="C63" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="30" t="s">
         <v>60</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -1692,40 +1693,40 @@
       <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D66" s="7"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
+      <c r="A67" s="31"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D67" s="7"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
-      <c r="B68" s="21"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="32"/>
       <c r="C68" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D68" s="7"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="19" t="s">
+      <c r="A69" s="31"/>
+      <c r="B69" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -1734,8 +1735,8 @@
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="21"/>
-      <c r="B70" s="21"/>
+      <c r="A70" s="32"/>
+      <c r="B70" s="32"/>
       <c r="C70" s="4" t="s">
         <v>53</v>
       </c>
@@ -1743,13 +1744,18 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D3:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A64:A70"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="B69:B70"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B9:B16"/>
@@ -1762,18 +1768,13 @@
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A64:A70"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D3:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1785,7 +1786,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D43" sqref="B18:D45"/>
     </sheetView>
   </sheetViews>
@@ -1798,11 +1799,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1819,64 +1820,64 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29" t="s">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1887,8 +1888,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1897,8 +1898,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1907,8 +1908,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
@@ -1917,8 +1918,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1927,8 +1928,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1937,8 +1938,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1947,8 +1948,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1971,296 +1972,296 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="40" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29" t="s">
+      <c r="A19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="38"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29" t="s">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="38"/>
+      <c r="D20" s="40"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29" t="s">
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29" t="s">
+      <c r="A22" s="48"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="38"/>
+      <c r="D22" s="40"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29" t="s">
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29" t="s">
+      <c r="A24" s="48"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="40" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29" t="s">
+      <c r="A25" s="48"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="38"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29" t="s">
+      <c r="A26" s="48"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="40" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="48" t="s">
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="38"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="48" t="s">
+      <c r="A28" s="48"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="38"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="48" t="s">
+      <c r="A29" s="48"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="40" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="48" t="s">
+      <c r="A30" s="48"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="38"/>
+      <c r="D30" s="40"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="48" t="s">
+      <c r="A31" s="48"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="40" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="48" t="s">
+      <c r="A32" s="48"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="38"/>
+      <c r="D32" s="40"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="48" t="s">
+      <c r="A33" s="48"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="38"/>
+      <c r="D33" s="40"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="48" t="s">
+      <c r="A34" s="48"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="40" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="48" t="s">
+      <c r="A35" s="48"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="38"/>
+      <c r="D35" s="40"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="48" t="s">
+      <c r="A36" s="48"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="40" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="48" t="s">
+      <c r="A37" s="48"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="38"/>
+      <c r="D37" s="40"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="48" t="s">
+      <c r="A38" s="48"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="40" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="48" t="s">
+      <c r="A39" s="48"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="38"/>
+      <c r="D39" s="40"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="49"/>
-      <c r="C40" s="48" t="s">
+      <c r="A40" s="48"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="38" t="s">
+      <c r="D40" s="40" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="48" t="s">
+      <c r="A41" s="48"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="38"/>
+      <c r="D41" s="40"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="48" t="s">
+      <c r="A42" s="48"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D42" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="48" t="s">
+      <c r="A43" s="48"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="38" t="s">
+      <c r="D43" s="40" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="49"/>
-      <c r="C44" s="48" t="s">
+      <c r="A44" s="48"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="38"/>
+      <c r="D44" s="40"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="48" t="s">
+      <c r="A45" s="48"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="38"/>
+      <c r="D45" s="40"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="40" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="29" t="s">
+      <c r="A47" s="31"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="38"/>
+      <c r="D47" s="40"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="29" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="38"/>
+      <c r="D48" s="40"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="34" t="s">
+      <c r="A49" s="31"/>
+      <c r="B49" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D49" s="39" t="s">
+      <c r="D49" s="41" t="s">
         <v>93</v>
       </c>
       <c r="E49">
@@ -2268,119 +2269,115 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="29" t="s">
+      <c r="A50" s="31"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="39"/>
+      <c r="D50" s="41"/>
       <c r="E50">
         <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="29" t="s">
+      <c r="A51" s="31"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D51" s="39"/>
+      <c r="D51" s="41"/>
       <c r="E51">
         <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="29" t="s">
+      <c r="A52" s="32"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="39"/>
+      <c r="D52" s="41"/>
       <c r="E52" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="36" t="s">
+      <c r="D53" s="17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="29" t="s">
+      <c r="A54" s="31"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="38" t="s">
+      <c r="D54" s="40" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="29" t="s">
+      <c r="A55" s="31"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="38"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="29" t="s">
+      <c r="A56" s="31"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="38"/>
+      <c r="D56" s="40"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="29" t="s">
+      <c r="A57" s="31"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D57" s="38"/>
+      <c r="D57" s="40"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
-      <c r="B58" s="34" t="s">
+      <c r="A58" s="31"/>
+      <c r="B58" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="29" t="s">
+      <c r="A59" s="32"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="14" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="B9:B16"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D43:D45"/>
@@ -2394,11 +2391,15 @@
     <mergeCell ref="D31:D33"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2410,7 +2411,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F23" sqref="F1:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2422,10 +2423,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E1" t="s">
@@ -2436,10 +2437,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
@@ -2450,10 +2451,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E3" t="s">
@@ -2464,10 +2465,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="18" t="s">
         <v>38</v>
       </c>
       <c r="E4" t="s">
@@ -2478,10 +2479,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="18" t="s">
         <v>38</v>
       </c>
       <c r="E5" t="s">
@@ -2492,10 +2493,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="18" t="s">
         <v>38</v>
       </c>
       <c r="E6" t="s">
@@ -2506,10 +2507,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="21" t="s">
         <v>64</v>
       </c>
       <c r="E7" t="s">
@@ -2520,10 +2521,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="21" t="s">
         <v>64</v>
       </c>
       <c r="E8" t="s">
@@ -2534,10 +2535,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E9" t="s">
@@ -2548,10 +2549,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E10" t="s">
@@ -2562,10 +2563,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E11" t="s">
@@ -2576,10 +2577,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="18" t="s">
         <v>83</v>
       </c>
       <c r="E12" t="s">
@@ -2590,10 +2591,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="18" t="s">
         <v>83</v>
       </c>
       <c r="E13" t="s">
@@ -2604,10 +2605,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="18" t="s">
         <v>84</v>
       </c>
       <c r="E14" t="s">
@@ -2618,10 +2619,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="18" t="s">
         <v>84</v>
       </c>
       <c r="E15" t="s">
@@ -2632,10 +2633,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="18" t="s">
         <v>84</v>
       </c>
       <c r="E16" t="s">
@@ -2646,10 +2647,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="21" t="s">
         <v>85</v>
       </c>
       <c r="E17" t="s">
@@ -2660,10 +2661,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="21" t="s">
         <v>85</v>
       </c>
       <c r="E18" t="s">
@@ -2674,10 +2675,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="21" t="s">
         <v>86</v>
       </c>
       <c r="E19" t="s">
@@ -2688,10 +2689,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="21" t="s">
         <v>86</v>
       </c>
       <c r="E20" t="s">
@@ -2702,10 +2703,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E21" t="s">
@@ -2716,10 +2717,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E22" t="s">
@@ -2730,10 +2731,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="18" t="s">
         <v>97</v>
       </c>
       <c r="E23" t="s">
@@ -2744,43 +2745,125 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="18" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="22" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="21" t="s">
         <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC845EB-521E-45A5-A5AE-B459C0F25D9A}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>